<commit_message>
added support for matches not played
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -111,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,14 +136,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF111111"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -219,7 +211,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,66 +224,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF111111"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -319,15 +251,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="25.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
   </cols>
@@ -1672,1358 +1604,1356 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="4" t="s">
+      <c r="P2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="I3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="N3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="U3" s="4" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="0" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="U4" s="4" t="s">
+      <c r="E4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="U5" s="4" t="s">
+      <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="4" t="s">
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U6" s="4" t="s">
+      <c r="Q6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="B7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="4" t="s">
+      <c r="H7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U7" s="4" t="s">
+      <c r="P7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="4" t="s">
+      <c r="I8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="D9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U9" s="4" t="s">
+      <c r="J9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="B10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="4" t="s">
+      <c r="K10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U10" s="4" t="s">
+      <c r="Q10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="4" t="s">
+      <c r="D11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U11" s="4" t="s">
+      <c r="L11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="4" t="s">
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="4" t="s">
+      <c r="M12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U12" s="4" t="s">
+      <c r="P12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="B13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="0" t="s">
         <v>20</v>
       </c>
       <c r="M13" s="3"/>
-      <c r="N13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="4" t="s">
+      <c r="N13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U13" s="4" t="s">
+      <c r="Q13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U13" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="4" t="s">
+      <c r="D14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="0" t="s">
         <v>20</v>
       </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="P14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U14" s="4" t="s">
+      <c r="Q14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="B15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="4" t="s">
+      <c r="J15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="0" t="s">
         <v>20</v>
       </c>
       <c r="O15" s="3"/>
-      <c r="P15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q15" s="4" t="s">
+      <c r="P15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T15" s="4" t="s">
+      <c r="R15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="U15" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="B16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="H16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="4" t="s">
+      <c r="J16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="0" t="s">
         <v>20</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R16" s="4" t="s">
+      <c r="Q16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U16" s="4" t="s">
+      <c r="S16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="U16" s="0" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P17" s="4" t="s">
+      <c r="B17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P17" s="0" t="s">
         <v>26</v>
       </c>
       <c r="Q17" s="3"/>
-      <c r="R17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U17" s="4" t="s">
+      <c r="R17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q18" s="4" t="s">
+      <c r="B18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="0" t="s">
         <v>20</v>
       </c>
       <c r="R18" s="3"/>
-      <c r="S18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U18" s="4" t="s">
+      <c r="S18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="4" t="s">
+      <c r="B19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R19" s="4" t="s">
+      <c r="P19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="0" t="s">
         <v>21</v>
       </c>
       <c r="S19" s="3"/>
-      <c r="T19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="4" t="s">
+      <c r="T19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U19" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S20" s="4" t="s">
+      <c r="D20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="0" t="s">
         <v>22</v>
       </c>
       <c r="T20" s="3"/>
-      <c r="U20" s="4" t="s">
+      <c r="U20" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T21" s="4" t="s">
+      <c r="B21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="T21" s="0" t="s">
         <v>20</v>
       </c>
       <c r="U21" s="3"/>

</xml_diff>